<commit_message>
Data, code, and results pop dynamics degus
</commit_message>
<xml_diff>
--- a/data/metafile_degu_markrecapture.xlsx
+++ b/data/metafile_degu_markrecapture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/anne_vandermarel_uc_cl/Documents/Degu/MS_populationcrash/degu-pop-crash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA1A35B6-E2CE-4F53-9083-D72A929C7979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{CA1A35B6-E2CE-4F53-9083-D72A929C7979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70BD66F9-EC96-4809-BC91-761631398A5D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4BC98F30-9C25-4C83-A29D-4ED1C0A7248A}"/>
+    <workbookView xWindow="3850" yWindow="2270" windowWidth="14400" windowHeight="7280" xr2:uid="{4BC98F30-9C25-4C83-A29D-4ED1C0A7248A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>column_name</t>
   </si>
@@ -119,9 +119,6 @@
     <t xml:space="preserve">date in yyyy-mm-dd format </t>
   </si>
   <si>
-    <t>julian date starting each year on 01-01 on 1</t>
-  </si>
-  <si>
     <t>in which trap the degu was trapped, Sh=Sherman, T=Tomahawk</t>
   </si>
   <si>
@@ -149,13 +146,28 @@
     <t>whether the vulva of the female is closed (0), semi-open (1), open (2)</t>
   </si>
   <si>
-    <t>breeding status of the females; 0 = nonbreeding, 1= definitely pregnant, 2 = definitely lactating, 3 = definitely postlactating, 4 = both pregnant and/or (post)lactating, 5 = unclear breeding status</t>
-  </si>
-  <si>
     <t>any notes</t>
   </si>
   <si>
     <t>from the trapping file notes, date of death because degus was found death</t>
+  </si>
+  <si>
+    <t>seasonkey</t>
+  </si>
+  <si>
+    <t>numeric variable that correponds with seasonid (fall_jun_2009=1, spring_oct_2009=2, …, spring_oct_2020=24)</t>
+  </si>
+  <si>
+    <t>julian date starting each year on 01-01 with 1</t>
+  </si>
+  <si>
+    <t>indicator variable of known death (0 = no known death, 1 = known to have died just before the sampling occasion)</t>
+  </si>
+  <si>
+    <t>breeding status of the females; 0 = nonbreeding, 1= definitely pregnant, 2 = definitely lactating, 3 = definitely postlactating meaning that the female was lactating within this spring season, 4 = both pregnant and/or (post)lactating, 5 = unclear breeding status</t>
+  </si>
+  <si>
+    <t>known_death</t>
   </si>
 </sst>
 </file>
@@ -507,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DDA34F-EB5F-498B-AFF8-B001BD7DB2C7}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,10 +548,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -560,122 +572,138 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>38</v>
+      <c r="B22" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>